<commit_message>
commit with all new changes
</commit_message>
<xml_diff>
--- a/Automation/data/login.xlsx
+++ b/Automation/data/login.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,44 +16,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>vks2f2f@gmail.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>http://www.google.com</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://www.facebook.com</t>
+  </si>
+  <si>
+    <t>TestScenario</t>
+  </si>
+  <si>
+    <t>GoogleLogin</t>
+  </si>
+  <si>
+    <t>FaceBookLogin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,19 +66,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -378,48 +365,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>